<commit_message>
feature: undo/redo 추가 /// fix: minor errors
</commit_message>
<xml_diff>
--- a/public/data/sample_org_data.xlsx
+++ b/public/data/sample_org_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaehyun/workspace/gaainkim0110.github.io/public/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F4EB965-F599-A143-ACA4-4673A5ED47A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7969F598-DC0B-6341-838F-8157FC6D9B5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="860" windowWidth="34200" windowHeight="21380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="34200" windowHeight="21380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample Org Data" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="132">
   <si>
     <t>No</t>
   </si>
@@ -486,6 +486,10 @@
   </si>
   <si>
     <t>준법감시그룹</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ORG002</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -870,16 +874,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:Q32"/>
+  <dimension ref="A1:Q33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" ht="17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -932,7 +935,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:17" hidden="1">
+    <row r="2" spans="1:17">
       <c r="A2">
         <v>1</v>
       </c>
@@ -966,9 +969,6 @@
       <c r="K2" t="s">
         <v>15</v>
       </c>
-      <c r="L2" t="s">
-        <v>55</v>
-      </c>
       <c r="M2" t="s">
         <v>22</v>
       </c>
@@ -976,7 +976,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:17" hidden="1">
+    <row r="3" spans="1:17">
       <c r="A3">
         <f>+A2+1</f>
         <v>2</v>
@@ -1024,7 +1024,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:17" hidden="1">
+    <row r="4" spans="1:17">
       <c r="A4">
         <f t="shared" ref="A4:A29" si="0">+A3+1</f>
         <v>3</v>
@@ -1072,7 +1072,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:17" hidden="1">
+    <row r="5" spans="1:17">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1120,7 +1120,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:17" hidden="1">
+    <row r="6" spans="1:17">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1168,7 +1168,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:17" hidden="1">
+    <row r="7" spans="1:17">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1216,7 +1216,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:17" hidden="1">
+    <row r="8" spans="1:17">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1264,7 +1264,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:17" hidden="1">
+    <row r="9" spans="1:17">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1312,7 +1312,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:17" hidden="1">
+    <row r="10" spans="1:17">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1345,7 +1345,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:17" hidden="1">
+    <row r="11" spans="1:17">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1393,7 +1393,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:17" hidden="1">
+    <row r="12" spans="1:17">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1441,7 +1441,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:17" hidden="1">
+    <row r="13" spans="1:17">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1483,7 +1483,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:17" hidden="1">
+    <row r="14" spans="1:17">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1528,7 +1528,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="15" spans="1:17" hidden="1">
+    <row r="15" spans="1:17">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1576,7 +1576,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="16" spans="1:17" hidden="1">
+    <row r="16" spans="1:17">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1624,7 +1624,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="1:15" hidden="1">
+    <row r="17" spans="1:15">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1672,7 +1672,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="1:15" hidden="1">
+    <row r="18" spans="1:15" ht="20" customHeight="1">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2284,7 +2284,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="31" spans="1:15" hidden="1">
+    <row r="31" spans="1:15">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2328,7 +2328,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="32" spans="1:15" hidden="1">
+    <row r="32" spans="1:15">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2369,14 +2369,52 @@
         <v>130</v>
       </c>
     </row>
+    <row r="33" spans="1:14">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" t="s">
+        <v>55</v>
+      </c>
+      <c r="E33" t="s">
+        <v>131</v>
+      </c>
+      <c r="F33" t="s">
+        <v>17</v>
+      </c>
+      <c r="G33" t="s">
+        <v>61</v>
+      </c>
+      <c r="H33" t="s">
+        <v>19</v>
+      </c>
+      <c r="I33" t="s">
+        <v>20</v>
+      </c>
+      <c r="J33" t="s">
+        <v>21</v>
+      </c>
+      <c r="K33" t="s">
+        <v>15</v>
+      </c>
+      <c r="L33" t="s">
+        <v>55</v>
+      </c>
+      <c r="M33" t="s">
+        <v>22</v>
+      </c>
+      <c r="N33" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:Q32" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="12">
-      <filters>
-        <filter val="IB본부"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:Q32" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>